<commit_message>
database storage diagram and working on getting historical data into database
</commit_message>
<xml_diff>
--- a/tech/database/equities/db-diagram.xlsx
+++ b/tech/database/equities/db-diagram.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/douglasterc/terc-capital/tech/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/douglasterc/terc-capital/tech/database/equities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C292643-1E63-A44E-A78A-6DEB62F1E583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136C4875-D653-4E4B-BD94-8CCE996A0689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17860" activeTab="1" xr2:uid="{B515DCDA-2F36-0A46-9A0C-33852D85EA0C}"/>
+    <workbookView xWindow="20240" yWindow="760" windowWidth="10000" windowHeight="17860" activeTab="1" xr2:uid="{B515DCDA-2F36-0A46-9A0C-33852D85EA0C}"/>
   </bookViews>
   <sheets>
     <sheet name="keys" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
   <si>
     <t>SCREENER</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>active</t>
+  </si>
+  <si>
+    <t>secure_id</t>
   </si>
 </sst>
 </file>
@@ -390,12 +393,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -417,16 +414,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -440,6 +437,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2861,8 +2864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1674C6F6-76D7-7344-A682-83CC8F31F6CD}">
   <dimension ref="B3:BB31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="BS31" sqref="BS31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="BG24" sqref="BG24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2871,56 +2874,56 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:54" x14ac:dyDescent="0.2">
-      <c r="AT3" s="18" t="s">
+      <c r="AT3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="AU3" s="19"/>
-      <c r="AV3" s="19"/>
-      <c r="AW3" s="19"/>
-      <c r="AX3" s="19"/>
-      <c r="AY3" s="19"/>
-      <c r="AZ3" s="19"/>
-      <c r="BA3" s="19"/>
-      <c r="BB3" s="20"/>
+      <c r="AU3" s="17"/>
+      <c r="AV3" s="17"/>
+      <c r="AW3" s="17"/>
+      <c r="AX3" s="17"/>
+      <c r="AY3" s="17"/>
+      <c r="AZ3" s="17"/>
+      <c r="BA3" s="17"/>
+      <c r="BB3" s="18"/>
     </row>
     <row r="4" spans="2:54" x14ac:dyDescent="0.2">
       <c r="AT4" s="10" t="s">
         <v>1</v>
       </c>
       <c r="AU4" s="11"/>
-      <c r="AV4" s="23" t="s">
+      <c r="AV4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="AW4" s="23"/>
-      <c r="AX4" s="23"/>
-      <c r="AY4" s="23"/>
-      <c r="AZ4" s="23"/>
-      <c r="BA4" s="23"/>
-      <c r="BB4" s="24"/>
+      <c r="AW4" s="19"/>
+      <c r="AX4" s="19"/>
+      <c r="AY4" s="19"/>
+      <c r="AZ4" s="19"/>
+      <c r="BA4" s="19"/>
+      <c r="BB4" s="20"/>
     </row>
     <row r="5" spans="2:54" x14ac:dyDescent="0.2">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="20"/>
-      <c r="AI5" s="18" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="18"/>
+      <c r="AI5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="AJ5" s="19"/>
-      <c r="AK5" s="19"/>
-      <c r="AL5" s="19"/>
-      <c r="AM5" s="19"/>
-      <c r="AN5" s="19"/>
-      <c r="AO5" s="19"/>
-      <c r="AP5" s="19"/>
-      <c r="AQ5" s="20"/>
+      <c r="AJ5" s="17"/>
+      <c r="AK5" s="17"/>
+      <c r="AL5" s="17"/>
+      <c r="AM5" s="17"/>
+      <c r="AN5" s="17"/>
+      <c r="AO5" s="17"/>
+      <c r="AP5" s="17"/>
+      <c r="AQ5" s="18"/>
       <c r="AT5" s="10"/>
       <c r="AU5" s="11"/>
       <c r="AV5" s="21" t="s">
@@ -2938,50 +2941,50 @@
         <v>1</v>
       </c>
       <c r="C6" s="11"/>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="24"/>
-      <c r="M6" s="18" t="s">
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="20"/>
+      <c r="M6" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="20"/>
-      <c r="X6" s="18" t="s">
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="18"/>
+      <c r="X6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="Y6" s="19"/>
-      <c r="Z6" s="19"/>
-      <c r="AA6" s="19"/>
-      <c r="AB6" s="19"/>
-      <c r="AC6" s="19"/>
-      <c r="AD6" s="19"/>
-      <c r="AE6" s="19"/>
-      <c r="AF6" s="20"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="17"/>
+      <c r="AA6" s="17"/>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="17"/>
+      <c r="AD6" s="17"/>
+      <c r="AE6" s="17"/>
+      <c r="AF6" s="18"/>
       <c r="AI6" s="10" t="s">
         <v>1</v>
       </c>
       <c r="AJ6" s="11"/>
-      <c r="AK6" s="23" t="s">
+      <c r="AK6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="AL6" s="23"/>
-      <c r="AM6" s="23"/>
-      <c r="AN6" s="23"/>
-      <c r="AO6" s="23"/>
-      <c r="AP6" s="23"/>
-      <c r="AQ6" s="24"/>
+      <c r="AL6" s="19"/>
+      <c r="AM6" s="19"/>
+      <c r="AN6" s="19"/>
+      <c r="AO6" s="19"/>
+      <c r="AP6" s="19"/>
+      <c r="AQ6" s="20"/>
       <c r="AT6" s="10"/>
       <c r="AU6" s="11"/>
       <c r="AV6" s="21" t="s">
@@ -3010,39 +3013,39 @@
         <v>1</v>
       </c>
       <c r="N7" s="11"/>
-      <c r="O7" s="23" t="s">
+      <c r="O7" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="24"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="20"/>
       <c r="X7" s="10" t="s">
         <v>1</v>
       </c>
       <c r="Y7" s="11"/>
-      <c r="Z7" s="23" t="s">
+      <c r="Z7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AA7" s="23"/>
-      <c r="AB7" s="23"/>
-      <c r="AC7" s="23"/>
-      <c r="AD7" s="23"/>
-      <c r="AE7" s="23"/>
-      <c r="AF7" s="24"/>
+      <c r="AA7" s="19"/>
+      <c r="AB7" s="19"/>
+      <c r="AC7" s="19"/>
+      <c r="AD7" s="19"/>
+      <c r="AE7" s="19"/>
+      <c r="AF7" s="20"/>
       <c r="AI7" s="10"/>
       <c r="AJ7" s="11"/>
-      <c r="AK7" s="12" t="s">
+      <c r="AK7" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="AL7" s="12"/>
-      <c r="AM7" s="12"/>
-      <c r="AN7" s="12"/>
-      <c r="AO7" s="12"/>
-      <c r="AP7" s="12"/>
-      <c r="AQ7" s="13"/>
+      <c r="AL7" s="27"/>
+      <c r="AM7" s="27"/>
+      <c r="AN7" s="27"/>
+      <c r="AO7" s="27"/>
+      <c r="AP7" s="27"/>
+      <c r="AQ7" s="28"/>
       <c r="AT7" s="10"/>
       <c r="AU7" s="11"/>
       <c r="AV7" s="21" t="s">
@@ -3100,15 +3103,15 @@
       <c r="AG8" s="1"/>
       <c r="AH8" s="2"/>
       <c r="AI8" s="6"/>
-      <c r="AK8" s="12" t="s">
+      <c r="AK8" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="AL8" s="12"/>
-      <c r="AM8" s="12"/>
-      <c r="AN8" s="12"/>
-      <c r="AO8" s="12"/>
-      <c r="AP8" s="12"/>
-      <c r="AQ8" s="13"/>
+      <c r="AL8" s="27"/>
+      <c r="AM8" s="27"/>
+      <c r="AN8" s="27"/>
+      <c r="AO8" s="27"/>
+      <c r="AP8" s="27"/>
+      <c r="AQ8" s="28"/>
       <c r="AR8" s="1"/>
       <c r="AS8" s="2"/>
       <c r="AT8" s="10"/>
@@ -3135,40 +3138,40 @@
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
       <c r="J9" s="22"/>
-      <c r="M9" s="14" t="s">
+      <c r="M9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N9" s="15"/>
-      <c r="O9" s="16" t="s">
+      <c r="N9" s="13"/>
+      <c r="O9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="17"/>
-      <c r="X9" s="14"/>
-      <c r="Y9" s="15"/>
-      <c r="Z9" s="16" t="s">
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="15"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="AA9" s="16"/>
-      <c r="AB9" s="16"/>
-      <c r="AC9" s="16"/>
-      <c r="AD9" s="16"/>
-      <c r="AE9" s="16"/>
-      <c r="AF9" s="17"/>
+      <c r="AA9" s="14"/>
+      <c r="AB9" s="14"/>
+      <c r="AC9" s="14"/>
+      <c r="AD9" s="14"/>
+      <c r="AE9" s="14"/>
+      <c r="AF9" s="15"/>
       <c r="AI9" s="6"/>
-      <c r="AK9" s="12" t="s">
+      <c r="AK9" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="AL9" s="12"/>
-      <c r="AM9" s="12"/>
-      <c r="AN9" s="12"/>
-      <c r="AO9" s="12"/>
-      <c r="AP9" s="12"/>
-      <c r="AQ9" s="13"/>
+      <c r="AL9" s="27"/>
+      <c r="AM9" s="27"/>
+      <c r="AN9" s="27"/>
+      <c r="AO9" s="27"/>
+      <c r="AP9" s="27"/>
+      <c r="AQ9" s="28"/>
       <c r="AT9" s="10"/>
       <c r="AU9" s="11"/>
       <c r="AV9" s="21" t="s">
@@ -3193,19 +3196,19 @@
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="22"/>
-      <c r="AI10" s="14" t="s">
+      <c r="AI10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AJ10" s="15"/>
-      <c r="AK10" s="16" t="s">
+      <c r="AJ10" s="13"/>
+      <c r="AK10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="AL10" s="16"/>
-      <c r="AM10" s="16"/>
-      <c r="AN10" s="16"/>
-      <c r="AO10" s="16"/>
-      <c r="AP10" s="16"/>
-      <c r="AQ10" s="17"/>
+      <c r="AL10" s="14"/>
+      <c r="AM10" s="14"/>
+      <c r="AN10" s="14"/>
+      <c r="AO10" s="14"/>
+      <c r="AP10" s="14"/>
+      <c r="AQ10" s="15"/>
       <c r="AT10" s="10"/>
       <c r="AU10" s="11"/>
       <c r="AV10" s="21" t="s">
@@ -3244,44 +3247,44 @@
       <c r="BB11" s="22"/>
     </row>
     <row r="12" spans="2:54" x14ac:dyDescent="0.2">
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16" t="s">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="17"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="15"/>
       <c r="AM12" s="8"/>
-      <c r="AT12" s="14"/>
-      <c r="AU12" s="15"/>
-      <c r="AV12" s="16" t="s">
+      <c r="AT12" s="12"/>
+      <c r="AU12" s="13"/>
+      <c r="AV12" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AW12" s="16"/>
-      <c r="AX12" s="16"/>
-      <c r="AY12" s="16"/>
-      <c r="AZ12" s="16"/>
-      <c r="BA12" s="16"/>
-      <c r="BB12" s="17"/>
+      <c r="AW12" s="14"/>
+      <c r="AX12" s="14"/>
+      <c r="AY12" s="14"/>
+      <c r="AZ12" s="14"/>
+      <c r="BA12" s="14"/>
+      <c r="BB12" s="15"/>
     </row>
     <row r="13" spans="2:54" x14ac:dyDescent="0.2">
       <c r="F13" s="6"/>
       <c r="I13" s="6"/>
-      <c r="S13" s="18" t="s">
+      <c r="S13" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="T13" s="19"/>
-      <c r="U13" s="19"/>
-      <c r="V13" s="19"/>
-      <c r="W13" s="19"/>
-      <c r="X13" s="19"/>
-      <c r="Y13" s="19"/>
-      <c r="Z13" s="19"/>
-      <c r="AA13" s="20"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="17"/>
+      <c r="Y13" s="17"/>
+      <c r="Z13" s="17"/>
+      <c r="AA13" s="18"/>
       <c r="AM13" s="8"/>
       <c r="AX13" s="1"/>
     </row>
@@ -3301,15 +3304,15 @@
         <v>1</v>
       </c>
       <c r="T14" s="11"/>
-      <c r="U14" s="23" t="s">
+      <c r="U14" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="V14" s="23"/>
-      <c r="W14" s="23"/>
-      <c r="X14" s="23"/>
-      <c r="Y14" s="23"/>
-      <c r="Z14" s="23"/>
-      <c r="AA14" s="24"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="19"/>
+      <c r="Y14" s="19"/>
+      <c r="Z14" s="19"/>
+      <c r="AA14" s="20"/>
       <c r="AM14" s="8"/>
       <c r="AX14" s="3"/>
     </row>
@@ -3329,17 +3332,17 @@
       <c r="Z15" s="21"/>
       <c r="AA15" s="22"/>
       <c r="AM15" s="8"/>
-      <c r="AT15" s="18" t="s">
+      <c r="AT15" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="AU15" s="19"/>
-      <c r="AV15" s="19"/>
-      <c r="AW15" s="19"/>
-      <c r="AX15" s="19"/>
-      <c r="AY15" s="19"/>
-      <c r="AZ15" s="19"/>
-      <c r="BA15" s="19"/>
-      <c r="BB15" s="20"/>
+      <c r="AU15" s="17"/>
+      <c r="AV15" s="17"/>
+      <c r="AW15" s="17"/>
+      <c r="AX15" s="17"/>
+      <c r="AY15" s="17"/>
+      <c r="AZ15" s="17"/>
+      <c r="BA15" s="17"/>
+      <c r="BB15" s="18"/>
     </row>
     <row r="16" spans="2:54" x14ac:dyDescent="0.2">
       <c r="F16" s="6"/>
@@ -3372,15 +3375,15 @@
         <v>1</v>
       </c>
       <c r="AU16" s="11"/>
-      <c r="AV16" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="AW16" s="23"/>
-      <c r="AX16" s="23"/>
-      <c r="AY16" s="23"/>
-      <c r="AZ16" s="23"/>
-      <c r="BA16" s="23"/>
-      <c r="BB16" s="24"/>
+      <c r="AV16" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AW16" s="19"/>
+      <c r="AX16" s="19"/>
+      <c r="AY16" s="19"/>
+      <c r="AZ16" s="19"/>
+      <c r="BA16" s="19"/>
+      <c r="BB16" s="20"/>
     </row>
     <row r="17" spans="5:54" x14ac:dyDescent="0.2">
       <c r="F17" s="3"/>
@@ -3395,10 +3398,10 @@
       <c r="Y17" s="21"/>
       <c r="Z17" s="21"/>
       <c r="AA17" s="22"/>
-      <c r="AT17" s="25" t="s">
+      <c r="AT17" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="AU17" s="26"/>
+      <c r="AU17" s="24"/>
       <c r="AV17" s="21" t="s">
         <v>6</v>
       </c>
@@ -3410,17 +3413,17 @@
       <c r="BB17" s="22"/>
     </row>
     <row r="18" spans="5:54" x14ac:dyDescent="0.2">
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="20"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="18"/>
       <c r="S18" s="10"/>
       <c r="T18" s="11"/>
       <c r="U18" s="21" t="s">
@@ -3432,8 +3435,8 @@
       <c r="Y18" s="21"/>
       <c r="Z18" s="21"/>
       <c r="AA18" s="22"/>
-      <c r="AT18" s="25"/>
-      <c r="AU18" s="26"/>
+      <c r="AT18" s="23"/>
+      <c r="AU18" s="24"/>
       <c r="AV18" s="21" t="s">
         <v>42</v>
       </c>
@@ -3449,15 +3452,15 @@
         <v>1</v>
       </c>
       <c r="F19" s="11"/>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="24"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="20"/>
       <c r="S19" s="10"/>
       <c r="T19" s="11"/>
       <c r="U19" s="21" t="s">
@@ -3469,8 +3472,8 @@
       <c r="Y19" s="21"/>
       <c r="Z19" s="21"/>
       <c r="AA19" s="22"/>
-      <c r="AT19" s="25"/>
-      <c r="AU19" s="26"/>
+      <c r="AT19" s="23"/>
+      <c r="AU19" s="24"/>
       <c r="AV19" s="21" t="s">
         <v>43</v>
       </c>
@@ -3504,8 +3507,8 @@
       <c r="Y20" s="21"/>
       <c r="Z20" s="21"/>
       <c r="AA20" s="22"/>
-      <c r="AT20" s="25"/>
-      <c r="AU20" s="26"/>
+      <c r="AT20" s="23"/>
+      <c r="AU20" s="24"/>
       <c r="AV20" s="21" t="s">
         <v>44</v>
       </c>
@@ -3541,28 +3544,28 @@
       <c r="Y21" s="21"/>
       <c r="Z21" s="21"/>
       <c r="AA21" s="22"/>
-      <c r="AF21" s="18" t="s">
+      <c r="AF21" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AG21" s="19"/>
-      <c r="AH21" s="19"/>
-      <c r="AI21" s="19"/>
-      <c r="AJ21" s="19"/>
-      <c r="AK21" s="19"/>
-      <c r="AL21" s="19"/>
-      <c r="AM21" s="19"/>
-      <c r="AN21" s="20"/>
-      <c r="AT21" s="27"/>
-      <c r="AU21" s="28"/>
-      <c r="AV21" s="16" t="s">
+      <c r="AG21" s="17"/>
+      <c r="AH21" s="17"/>
+      <c r="AI21" s="17"/>
+      <c r="AJ21" s="17"/>
+      <c r="AK21" s="17"/>
+      <c r="AL21" s="17"/>
+      <c r="AM21" s="17"/>
+      <c r="AN21" s="18"/>
+      <c r="AT21" s="25"/>
+      <c r="AU21" s="26"/>
+      <c r="AV21" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AW21" s="16"/>
-      <c r="AX21" s="16"/>
-      <c r="AY21" s="16"/>
-      <c r="AZ21" s="16"/>
-      <c r="BA21" s="16"/>
-      <c r="BB21" s="17"/>
+      <c r="AW21" s="14"/>
+      <c r="AX21" s="14"/>
+      <c r="AY21" s="14"/>
+      <c r="AZ21" s="14"/>
+      <c r="BA21" s="14"/>
+      <c r="BB21" s="15"/>
     </row>
     <row r="22" spans="5:54" x14ac:dyDescent="0.2">
       <c r="E22" s="10"/>
@@ -3576,30 +3579,30 @@
       <c r="K22" s="21"/>
       <c r="L22" s="21"/>
       <c r="M22" s="22"/>
-      <c r="S22" s="14"/>
-      <c r="T22" s="15"/>
-      <c r="U22" s="16" t="s">
+      <c r="S22" s="12"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="V22" s="16"/>
-      <c r="W22" s="16"/>
-      <c r="X22" s="16"/>
-      <c r="Y22" s="16"/>
-      <c r="Z22" s="16"/>
-      <c r="AA22" s="17"/>
+      <c r="V22" s="14"/>
+      <c r="W22" s="14"/>
+      <c r="X22" s="14"/>
+      <c r="Y22" s="14"/>
+      <c r="Z22" s="14"/>
+      <c r="AA22" s="15"/>
       <c r="AF22" s="10" t="s">
         <v>1</v>
       </c>
       <c r="AG22" s="11"/>
-      <c r="AH22" s="23" t="s">
+      <c r="AH22" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="AI22" s="23"/>
-      <c r="AJ22" s="23"/>
-      <c r="AK22" s="23"/>
-      <c r="AL22" s="23"/>
-      <c r="AM22" s="23"/>
-      <c r="AN22" s="24"/>
+      <c r="AI22" s="19"/>
+      <c r="AJ22" s="19"/>
+      <c r="AK22" s="19"/>
+      <c r="AL22" s="19"/>
+      <c r="AM22" s="19"/>
+      <c r="AN22" s="20"/>
     </row>
     <row r="23" spans="5:54" x14ac:dyDescent="0.2">
       <c r="E23" s="10"/>
@@ -3669,17 +3672,17 @@
       <c r="K25" s="21"/>
       <c r="L25" s="21"/>
       <c r="M25" s="22"/>
-      <c r="S25" s="18" t="s">
+      <c r="S25" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="T25" s="19"/>
-      <c r="U25" s="19"/>
-      <c r="V25" s="19"/>
-      <c r="W25" s="19"/>
-      <c r="X25" s="19"/>
-      <c r="Y25" s="19"/>
-      <c r="Z25" s="19"/>
-      <c r="AA25" s="20"/>
+      <c r="T25" s="17"/>
+      <c r="U25" s="17"/>
+      <c r="V25" s="17"/>
+      <c r="W25" s="17"/>
+      <c r="X25" s="17"/>
+      <c r="Y25" s="17"/>
+      <c r="Z25" s="17"/>
+      <c r="AA25" s="18"/>
       <c r="AC25" s="8"/>
       <c r="AF25" s="10"/>
       <c r="AG25" s="11"/>
@@ -3709,15 +3712,15 @@
         <v>1</v>
       </c>
       <c r="T26" s="11"/>
-      <c r="U26" s="23" t="s">
+      <c r="U26" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="V26" s="23"/>
-      <c r="W26" s="23"/>
-      <c r="X26" s="23"/>
-      <c r="Y26" s="23"/>
-      <c r="Z26" s="23"/>
-      <c r="AA26" s="24"/>
+      <c r="V26" s="19"/>
+      <c r="W26" s="19"/>
+      <c r="X26" s="19"/>
+      <c r="Y26" s="19"/>
+      <c r="Z26" s="19"/>
+      <c r="AA26" s="20"/>
       <c r="AC26" s="8"/>
       <c r="AF26" s="10"/>
       <c r="AG26" s="11"/>
@@ -3841,17 +3844,17 @@
       <c r="AN29" s="22"/>
     </row>
     <row r="30" spans="5:54" x14ac:dyDescent="0.2">
-      <c r="E30" s="14"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="16" t="s">
+      <c r="E30" s="12"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="17"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="15"/>
       <c r="S30" s="10"/>
       <c r="T30" s="11"/>
       <c r="U30" s="21" t="s">
@@ -3876,40 +3879,146 @@
       <c r="AN30" s="22"/>
     </row>
     <row r="31" spans="5:54" x14ac:dyDescent="0.2">
-      <c r="S31" s="14"/>
-      <c r="T31" s="15"/>
-      <c r="U31" s="16" t="s">
+      <c r="S31" s="12"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="V31" s="16"/>
-      <c r="W31" s="16"/>
-      <c r="X31" s="16"/>
-      <c r="Y31" s="16"/>
-      <c r="Z31" s="16"/>
-      <c r="AA31" s="17"/>
-      <c r="AF31" s="14"/>
-      <c r="AG31" s="15"/>
-      <c r="AH31" s="16" t="s">
+      <c r="V31" s="14"/>
+      <c r="W31" s="14"/>
+      <c r="X31" s="14"/>
+      <c r="Y31" s="14"/>
+      <c r="Z31" s="14"/>
+      <c r="AA31" s="15"/>
+      <c r="AF31" s="12"/>
+      <c r="AG31" s="13"/>
+      <c r="AH31" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="AI31" s="16"/>
-      <c r="AJ31" s="16"/>
-      <c r="AK31" s="16"/>
-      <c r="AL31" s="16"/>
-      <c r="AM31" s="16"/>
-      <c r="AN31" s="17"/>
+      <c r="AI31" s="14"/>
+      <c r="AJ31" s="14"/>
+      <c r="AK31" s="14"/>
+      <c r="AL31" s="14"/>
+      <c r="AM31" s="14"/>
+      <c r="AN31" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="148">
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:J12"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="AI7:AJ7"/>
+    <mergeCell ref="AK7:AQ7"/>
+    <mergeCell ref="AK8:AQ8"/>
+    <mergeCell ref="AK9:AQ9"/>
+    <mergeCell ref="AF31:AG31"/>
+    <mergeCell ref="AH31:AN31"/>
+    <mergeCell ref="S25:AA25"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="U29:AA29"/>
+    <mergeCell ref="S30:T30"/>
+    <mergeCell ref="U30:AA30"/>
+    <mergeCell ref="S31:T31"/>
+    <mergeCell ref="U31:AA31"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="U26:AA26"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="U27:AA27"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="U28:AA28"/>
+    <mergeCell ref="AF26:AG26"/>
+    <mergeCell ref="AH26:AN26"/>
+    <mergeCell ref="AF27:AG27"/>
+    <mergeCell ref="AH27:AN27"/>
+    <mergeCell ref="AF28:AG28"/>
+    <mergeCell ref="M6:U6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:U7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:U8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:U9"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="U20:AA20"/>
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="Z7:AF7"/>
+    <mergeCell ref="X8:Y8"/>
+    <mergeCell ref="Z8:AF8"/>
+    <mergeCell ref="X9:Y9"/>
+    <mergeCell ref="Z9:AF9"/>
+    <mergeCell ref="X6:AF6"/>
+    <mergeCell ref="AV10:BB10"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="U17:AA17"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="U18:AA18"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="U19:AA19"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="U14:AA14"/>
+    <mergeCell ref="S13:AA13"/>
+    <mergeCell ref="AT15:BB15"/>
+    <mergeCell ref="AT16:AU16"/>
+    <mergeCell ref="AV16:BB16"/>
+    <mergeCell ref="AT17:AU17"/>
+    <mergeCell ref="AV17:BB17"/>
+    <mergeCell ref="AV18:BB18"/>
+    <mergeCell ref="AV19:BB19"/>
+    <mergeCell ref="AT9:AU9"/>
+    <mergeCell ref="AT10:AU10"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="U22:AA22"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="U15:AA15"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="U16:AA16"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="U21:AA21"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:M25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:M26"/>
+    <mergeCell ref="G29:M29"/>
+    <mergeCell ref="AI5:AQ5"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="AK6:AQ6"/>
+    <mergeCell ref="AI10:AJ10"/>
+    <mergeCell ref="AK10:AQ10"/>
+    <mergeCell ref="AF21:AN21"/>
+    <mergeCell ref="AF22:AG22"/>
+    <mergeCell ref="AH22:AN22"/>
+    <mergeCell ref="AF29:AG29"/>
+    <mergeCell ref="AH29:AN29"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="AH28:AN28"/>
+    <mergeCell ref="AF23:AG23"/>
+    <mergeCell ref="AH23:AN23"/>
+    <mergeCell ref="AF24:AG24"/>
+    <mergeCell ref="AH24:AN24"/>
+    <mergeCell ref="AF25:AG25"/>
+    <mergeCell ref="AV6:BB6"/>
+    <mergeCell ref="AV7:BB7"/>
+    <mergeCell ref="AV8:BB8"/>
+    <mergeCell ref="AV9:BB9"/>
+    <mergeCell ref="G21:M21"/>
+    <mergeCell ref="G22:M22"/>
+    <mergeCell ref="G23:M23"/>
+    <mergeCell ref="G24:M24"/>
+    <mergeCell ref="D11:J11"/>
+    <mergeCell ref="D6:J6"/>
+    <mergeCell ref="D7:J7"/>
+    <mergeCell ref="AT11:AU11"/>
+    <mergeCell ref="AV11:BB11"/>
+    <mergeCell ref="AT12:AU12"/>
+    <mergeCell ref="AV12:BB12"/>
+    <mergeCell ref="AT18:AU18"/>
+    <mergeCell ref="AT19:AU19"/>
+    <mergeCell ref="AT20:AU20"/>
+    <mergeCell ref="AT21:AU21"/>
+    <mergeCell ref="AV20:BB20"/>
+    <mergeCell ref="AV21:BB21"/>
+    <mergeCell ref="AT6:AU6"/>
+    <mergeCell ref="AT7:AU7"/>
+    <mergeCell ref="AT8:AU8"/>
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="G30:M30"/>
@@ -3934,121 +4043,15 @@
     <mergeCell ref="AF30:AG30"/>
     <mergeCell ref="AH30:AN30"/>
     <mergeCell ref="AH25:AN25"/>
-    <mergeCell ref="AV6:BB6"/>
-    <mergeCell ref="AV7:BB7"/>
-    <mergeCell ref="AV8:BB8"/>
-    <mergeCell ref="AV9:BB9"/>
-    <mergeCell ref="G21:M21"/>
-    <mergeCell ref="G22:M22"/>
-    <mergeCell ref="G23:M23"/>
-    <mergeCell ref="G24:M24"/>
-    <mergeCell ref="D11:J11"/>
-    <mergeCell ref="D6:J6"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:M25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:M26"/>
-    <mergeCell ref="G29:M29"/>
-    <mergeCell ref="AI5:AQ5"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="AK6:AQ6"/>
-    <mergeCell ref="AI10:AJ10"/>
-    <mergeCell ref="AK10:AQ10"/>
-    <mergeCell ref="AT11:AU11"/>
-    <mergeCell ref="AV11:BB11"/>
-    <mergeCell ref="AT12:AU12"/>
-    <mergeCell ref="AV12:BB12"/>
-    <mergeCell ref="AT18:AU18"/>
-    <mergeCell ref="AT19:AU19"/>
-    <mergeCell ref="AT20:AU20"/>
-    <mergeCell ref="AT21:AU21"/>
-    <mergeCell ref="AV20:BB20"/>
-    <mergeCell ref="AV21:BB21"/>
-    <mergeCell ref="AF21:AN21"/>
-    <mergeCell ref="AF22:AG22"/>
-    <mergeCell ref="AH22:AN22"/>
-    <mergeCell ref="AF29:AG29"/>
-    <mergeCell ref="AH29:AN29"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="AT6:AU6"/>
-    <mergeCell ref="AT7:AU7"/>
-    <mergeCell ref="AT8:AU8"/>
-    <mergeCell ref="AT9:AU9"/>
-    <mergeCell ref="AT10:AU10"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="U22:AA22"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="U15:AA15"/>
-    <mergeCell ref="S16:T16"/>
-    <mergeCell ref="U16:AA16"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="U21:AA21"/>
-    <mergeCell ref="AV10:BB10"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="U17:AA17"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="U18:AA18"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="U19:AA19"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="U14:AA14"/>
-    <mergeCell ref="S13:AA13"/>
-    <mergeCell ref="AT15:BB15"/>
-    <mergeCell ref="AT16:AU16"/>
-    <mergeCell ref="AV16:BB16"/>
-    <mergeCell ref="AT17:AU17"/>
-    <mergeCell ref="AV17:BB17"/>
-    <mergeCell ref="AV18:BB18"/>
-    <mergeCell ref="AV19:BB19"/>
-    <mergeCell ref="AH28:AN28"/>
-    <mergeCell ref="AF23:AG23"/>
-    <mergeCell ref="AH23:AN23"/>
-    <mergeCell ref="AF24:AG24"/>
-    <mergeCell ref="AH24:AN24"/>
-    <mergeCell ref="AF25:AG25"/>
-    <mergeCell ref="M6:U6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:U7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:U8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:U9"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="U20:AA20"/>
-    <mergeCell ref="X7:Y7"/>
-    <mergeCell ref="Z7:AF7"/>
-    <mergeCell ref="X8:Y8"/>
-    <mergeCell ref="Z8:AF8"/>
-    <mergeCell ref="X9:Y9"/>
-    <mergeCell ref="Z9:AF9"/>
-    <mergeCell ref="X6:AF6"/>
-    <mergeCell ref="AI7:AJ7"/>
-    <mergeCell ref="AK7:AQ7"/>
-    <mergeCell ref="AK8:AQ8"/>
-    <mergeCell ref="AK9:AQ9"/>
-    <mergeCell ref="AF31:AG31"/>
-    <mergeCell ref="AH31:AN31"/>
-    <mergeCell ref="S25:AA25"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="U29:AA29"/>
-    <mergeCell ref="S30:T30"/>
-    <mergeCell ref="U30:AA30"/>
-    <mergeCell ref="S31:T31"/>
-    <mergeCell ref="U31:AA31"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="U26:AA26"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="U27:AA27"/>
-    <mergeCell ref="S28:T28"/>
-    <mergeCell ref="U28:AA28"/>
-    <mergeCell ref="AF26:AG26"/>
-    <mergeCell ref="AH26:AN26"/>
-    <mergeCell ref="AF27:AG27"/>
-    <mergeCell ref="AH27:AN27"/>
-    <mergeCell ref="AF28:AG28"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:J12"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>